<commit_message>
record front end click event
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
   <si>
     <t>dapp后端：存储数据</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -306,6 +306,10 @@
   </si>
   <si>
     <t>提现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(x-Rx)^2+(y-Ry)^2&lt;R^2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -677,6 +681,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,21 +725,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3902,10 +3906,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3921,35 +3925,35 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="48" t="s">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="40" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="36"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3972,7 +3976,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="46"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -3993,7 +3997,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="46"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
@@ -4014,7 +4018,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4035,7 +4039,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -4058,7 +4062,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="46"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -4079,7 +4083,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="47"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="9" t="s">
         <v>24</v>
       </c>
@@ -4100,7 +4104,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -4126,7 +4130,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="46"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
@@ -4147,7 +4151,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
@@ -4168,7 +4172,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="35" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4191,7 +4195,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A16" s="46"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -4212,7 +4216,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="46"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
@@ -4233,7 +4237,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="46"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -4254,7 +4258,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="46"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
@@ -4275,7 +4279,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="46"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
@@ -4296,7 +4300,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="46"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
@@ -4317,7 +4321,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="47"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
@@ -4408,26 +4412,31 @@
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A92" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A94" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A3:B4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A22"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A3:B4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add back end verify
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="问题描述" sheetId="2" r:id="rId1"/>
     <sheet name="表格对比" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="时间轴" sheetId="5" r:id="rId3"/>
+    <sheet name="遗留" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="84">
   <si>
     <t>dapp后端：存储数据</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -281,36 +282,74 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用户选项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>||</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>username</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>logout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>registration</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>提现</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(x-Rx)^2+(y-Ry)^2&lt;R^2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>(x-Rx)^2+(y-Ry)^2&lt;R^2+50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.1. 空间维度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.2. 时间维度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.2.1.目标持续：1.2s</t>
+  </si>
+  <si>
+    <t>3.2.2.1.目标持续：1.2s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.2.2.目标周期：0.7s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.2.3.结束延迟：0.55s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.2.2.目标周期：0.7s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.2.3.结束延迟：0.55s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0              1.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7             1.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.4              2.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.7*i&lt;t&lt;0.7*i+1.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2*2-0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2*3-0.5*2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2*n-0.5*(n-1)+0.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ActionDispatch::Cookies::CookieOverflow</t>
   </si>
 </sst>
 </file>
@@ -593,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -681,21 +720,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -725,6 +749,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3526,6 +3568,146 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="直接连接符 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="704850"/>
+          <a:ext cx="1390650" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直接连接符 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781050" y="866775"/>
+          <a:ext cx="1390650" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直接连接符 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1514475" y="1209675"/>
+          <a:ext cx="1390650" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3906,10 +4088,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView showGridLines="0" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3925,35 +4107,35 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="38" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="41"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="45" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3976,7 +4158,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="36"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -3997,7 +4179,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="36"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
@@ -4018,7 +4200,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4039,7 +4221,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="45" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -4062,7 +4244,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="36"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -4083,7 +4265,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="9" t="s">
         <v>24</v>
       </c>
@@ -4104,7 +4286,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="45" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -4130,7 +4312,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="36"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
@@ -4151,7 +4333,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
@@ -4172,7 +4354,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="45" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4195,7 +4377,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A16" s="36"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -4216,7 +4398,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="36"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
@@ -4237,7 +4419,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="36"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -4258,7 +4440,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="36"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
@@ -4279,7 +4461,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="36"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
@@ -4300,7 +4482,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="36"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
@@ -4321,7 +4503,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
@@ -4352,7 +4534,7 @@
       </c>
       <c r="B25" s="33"/>
       <c r="G25" s="33" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H25" s="33"/>
     </row>
@@ -4410,33 +4592,63 @@
         <v>65</v>
       </c>
     </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A90" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>73</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A92" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A95" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A97" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A98" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="A3:B4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A22"/>
-    <mergeCell ref="C3:C4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4447,50 +4659,101 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>69</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B6" s="50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C7" s="50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <f>1.2*3-0.5*2</f>
+        <v>2.5999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <f>12-4.5</f>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add fe onchain method
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="问题描述" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="85">
   <si>
     <t>dapp后端：存储数据</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -270,10 +270,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.后端提现验证模块</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4.1.sessionid+分数+提现金额</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -350,6 +346,14 @@
   </si>
   <si>
     <t>ActionDispatch::Cookies::CookieOverflow</t>
+  </si>
+  <si>
+    <t>4.后端提现验证模块(安装钱包&amp;&amp;数据库分数==链上分数)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.同步数据（安装钱包&amp;&amp;数据库分数&gt;链上分数)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -720,6 +724,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -749,24 +771,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4088,10 +4092,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4107,35 +4111,35 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="48" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="41" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="36"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -4158,7 +4162,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="46"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -4179,7 +4183,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="46"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
@@ -4200,7 +4204,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4221,7 +4225,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -4244,7 +4248,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="46"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -4265,7 +4269,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="47"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="9" t="s">
         <v>24</v>
       </c>
@@ -4286,7 +4290,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -4312,7 +4316,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="46"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
@@ -4333,7 +4337,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
@@ -4354,7 +4358,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="36" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4377,7 +4381,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A16" s="46"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -4398,7 +4402,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="46"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
@@ -4419,7 +4423,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="46"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -4440,7 +4444,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="46"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
@@ -4461,7 +4465,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="46"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
@@ -4482,7 +4486,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="46"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
@@ -4503,7 +4507,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="47"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
@@ -4534,7 +4538,7 @@
       </c>
       <c r="B25" s="33"/>
       <c r="G25" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H25" s="33"/>
     </row>
@@ -4589,66 +4593,71 @@
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A97" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>64</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A99" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A101" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A3:B4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A22"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A3:B4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4662,39 +4671,39 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="50" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B6" s="35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B6" s="50" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C7" s="35" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C7" s="50" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -4704,12 +4713,12 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -4720,7 +4729,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
@@ -4741,15 +4750,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add withdraw function and mask
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="问题描述" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="86">
   <si>
     <t>dapp后端：存储数据</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -345,14 +345,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ActionDispatch::Cookies::CookieOverflow</t>
-  </si>
-  <si>
     <t>4.后端提现验证模块(安装钱包&amp;&amp;数据库分数==链上分数)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5.同步数据（安装钱包&amp;&amp;数据库分数&gt;链上分数)</t>
+    <t>5.同步链上数据（安装钱包&amp;&amp;数据库分数&gt;链上分数)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.ActionDispatch::Cookies::CookieOverflow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.取消交易</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -727,21 +732,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -771,6 +761,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4094,8 +4099,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView showGridLines="0" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4111,35 +4116,35 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="39" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="36" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="46" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -4162,7 +4167,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="37"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -4183,7 +4188,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
@@ -4204,7 +4209,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="38"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4225,7 +4230,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="46" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -4248,7 +4253,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="37"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -4269,7 +4274,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="9" t="s">
         <v>24</v>
       </c>
@@ -4290,7 +4295,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -4316,7 +4321,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="37"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
@@ -4337,7 +4342,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="38"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
@@ -4358,7 +4363,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="46" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4381,7 +4386,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A16" s="37"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -4402,7 +4407,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="37"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
@@ -4423,7 +4428,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="37"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -4444,7 +4449,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="37"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
@@ -4465,7 +4470,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="37"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
@@ -4486,7 +4491,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="37"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
@@ -4507,7 +4512,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="38"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
@@ -4633,7 +4638,7 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.15">
@@ -4643,21 +4648,21 @@
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="A3:B4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A22"/>
-    <mergeCell ref="C3:C4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4748,17 +4753,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix cookie overflow bug
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="87">
   <si>
     <t>dapp后端：存储数据</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -358,6 +358,10 @@
   </si>
   <si>
     <t>2.取消交易</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.后端数据库保存score？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -732,6 +736,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -761,21 +780,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4099,8 +4103,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView showGridLines="0" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4116,35 +4120,35 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="49" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="41" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="37"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -4167,7 +4171,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="47"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -4188,7 +4192,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="47"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
@@ -4209,7 +4213,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4230,7 +4234,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -4253,7 +4257,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="47"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -4274,7 +4278,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="48"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="9" t="s">
         <v>24</v>
       </c>
@@ -4295,7 +4299,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -4321,7 +4325,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="47"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
@@ -4342,7 +4346,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="48"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
@@ -4363,7 +4367,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="36" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4386,7 +4390,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A16" s="47"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -4407,7 +4411,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="47"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
@@ -4428,7 +4432,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="47"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -4449,7 +4453,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="47"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
@@ -4470,7 +4474,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="47"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
@@ -4491,7 +4495,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="47"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
@@ -4512,7 +4516,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="48"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
@@ -4653,16 +4657,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A3:B4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A22"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A3:B4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4676,7 +4680,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4753,22 +4757,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="33" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <f>39*60</f>
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <f>81*30</f>
+        <v>2430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>